<commit_message>
Merged the process IDs in
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.0.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331891AE-F453-481A-91FD-4538B5B585D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCEB4AE-10B3-4786-8DCF-E2D9A2D8FC16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11895" yWindow="660" windowWidth="25470" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="471">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1038,12 +1038,6 @@
     <t>TICC-180</t>
   </si>
   <si>
-    <t>cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:01:1.0</t>
-  </si>
-  <si>
-    <t>cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:02:1.0</t>
-  </si>
-  <si>
     <t>cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:09:1.0</t>
   </si>
   <si>
@@ -1465,6 +1459,29 @@
   </si>
   <si>
     <t>TICC-54</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:01:1.0
+cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:03:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:02:1.0
+cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:04:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:01:1.0
+cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:02:1.0
+cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:03:1.0
+cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:04:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:01:1.0
+cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:03:1.0
+cenbii-procid-ubl::urn:fdc:bits.no:2017:profile:09:1.0</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:fdc:anskaffelser.no:2019:ehf:postaward:g3:09:1.0
+cenbii-procid-ubl::urn:fdc:anskaffelser.no:2019:ehf:postaward:g3:02:1.0</t>
   </si>
 </sst>
 </file>
@@ -2023,9 +2040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A148" sqref="A148:XFD148"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I109" sqref="I109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,16 +2073,16 @@
         <v>151</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>134</v>
@@ -2097,7 +2114,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F2" s="7">
         <v>2</v>
@@ -2130,7 +2147,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F3" s="7">
         <v>2</v>
@@ -2163,7 +2180,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F4" s="7">
         <v>2</v>
@@ -2196,7 +2213,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F5" s="7">
         <v>2</v>
@@ -2229,7 +2246,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F6" s="7">
         <v>2</v>
@@ -2262,7 +2279,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F7" s="7">
         <v>2</v>
@@ -2295,7 +2312,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F8" s="7">
         <v>7</v>
@@ -2328,7 +2345,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>
@@ -2349,7 +2366,7 @@
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>56</v>
@@ -2361,13 +2378,13 @@
         <v>27</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F10" s="7">
         <v>3</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I10" s="6" t="b">
         <f>TRUE</f>
@@ -2397,7 +2414,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F11" s="7">
         <v>7</v>
@@ -2430,7 +2447,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
@@ -2463,7 +2480,7 @@
         <v>27</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F13" s="7">
         <v>7</v>
@@ -2496,7 +2513,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F14" s="7">
         <v>2</v>
@@ -2529,7 +2546,7 @@
         <v>17</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F15" s="7">
         <v>2</v>
@@ -2562,7 +2579,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F16" s="7">
         <v>2</v>
@@ -2595,7 +2612,7 @@
         <v>27</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F17" s="7">
         <v>7</v>
@@ -2628,7 +2645,7 @@
         <v>27</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F18" s="7">
         <v>7</v>
@@ -2661,7 +2678,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F19" s="7">
         <v>7</v>
@@ -2694,7 +2711,7 @@
         <v>16</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F20" s="7">
         <v>7</v>
@@ -2727,7 +2744,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F21" s="7">
         <v>7</v>
@@ -2760,7 +2777,7 @@
         <v>16</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F22" s="7">
         <v>7</v>
@@ -2793,7 +2810,7 @@
         <v>16</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F23" s="7">
         <v>7</v>
@@ -2826,7 +2843,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F24" s="7">
         <v>7</v>
@@ -2859,7 +2876,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F25" s="7">
         <v>2</v>
@@ -2889,7 +2906,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I26" s="6" t="b">
         <f>FALSE</f>
@@ -2916,7 +2933,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F27" s="7">
         <v>7</v>
@@ -2937,7 +2954,7 @@
     </row>
     <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>56</v>
@@ -2949,13 +2966,13 @@
         <v>27</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F28" s="7">
         <v>3</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I28" s="6" t="b">
         <f>TRUE</f>
@@ -2985,7 +3002,7 @@
         <v>3</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F29" s="7">
         <v>7</v>
@@ -3018,7 +3035,7 @@
         <v>27</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F30" s="7">
         <v>7</v>
@@ -3051,7 +3068,7 @@
         <v>27</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F31" s="7">
         <v>7</v>
@@ -3084,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I32" s="6" t="b">
         <f>TRUE</f>
@@ -3114,7 +3131,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I33" s="6" t="b">
         <f>TRUE</f>
@@ -3144,7 +3161,7 @@
         <v>3</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I34" s="6" t="b">
         <f>FALSE</f>
@@ -3159,7 +3176,7 @@
     </row>
     <row r="35" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>56</v>
@@ -3171,13 +3188,13 @@
         <v>3</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F35" s="7" t="s">
         <v>324</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I35" s="6" t="b">
         <f>FALSE</f>
@@ -3198,16 +3215,16 @@
         <v>56</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I36" s="6" t="b">
         <f>FALSE</f>
@@ -3234,7 +3251,7 @@
         <v>3</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I37" s="6" t="b">
         <f>TRUE</f>
@@ -3264,7 +3281,7 @@
         <v>3</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I38" s="6" t="b">
         <f>TRUE</f>
@@ -3294,7 +3311,7 @@
         <v>3</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I39" s="6" t="b">
         <f>TRUE</f>
@@ -3324,7 +3341,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I40" s="6" t="b">
         <f>TRUE</f>
@@ -3354,7 +3371,7 @@
         <v>3</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I41" s="6" t="b">
         <f>TRUE</f>
@@ -3384,7 +3401,7 @@
         <v>3</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I42" s="6" t="b">
         <f>TRUE</f>
@@ -3414,7 +3431,7 @@
         <v>3</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I43" s="6" t="b">
         <f>TRUE</f>
@@ -3444,13 +3461,13 @@
         <v>3</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F44" s="7">
         <v>5</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I44" s="6" t="b">
         <f>FALSE</f>
@@ -3477,13 +3494,13 @@
         <v>3</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F45" s="7">
         <v>5</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I45" s="6" t="b">
         <f>FALSE</f>
@@ -3510,13 +3527,13 @@
         <v>3</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F46" s="7">
         <v>5</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I46" s="6" t="b">
         <f>FALSE</f>
@@ -3543,10 +3560,10 @@
         <v>3</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I47" s="6" t="b">
         <f>FALSE</f>
@@ -3573,10 +3590,10 @@
         <v>3</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I48" s="6" t="b">
         <f>FALSE</f>
@@ -3603,10 +3620,10 @@
         <v>3</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I49" s="6" t="b">
         <f>FALSE</f>
@@ -3633,10 +3650,10 @@
         <v>3</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I50" s="6" t="b">
         <f>FALSE</f>
@@ -3663,7 +3680,7 @@
         <v>4</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F51" s="7">
         <v>7</v>
@@ -3696,7 +3713,7 @@
         <v>4</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I52" s="6" t="b">
         <f>TRUE</f>
@@ -3726,7 +3743,7 @@
         <v>4</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I53" s="6" t="b">
         <f>TRUE</f>
@@ -3756,7 +3773,7 @@
         <v>4</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I54" s="6" t="b">
         <f>TRUE</f>
@@ -3786,7 +3803,7 @@
         <v>4</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I55" s="6" t="b">
         <f>TRUE</f>
@@ -3816,7 +3833,7 @@
         <v>4</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I56" s="6" t="b">
         <f>TRUE</f>
@@ -3846,7 +3863,7 @@
         <v>4</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I57" s="6" t="b">
         <f>TRUE</f>
@@ -3876,7 +3893,7 @@
         <v>4</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I58" s="6" t="b">
         <f>TRUE</f>
@@ -3906,7 +3923,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I59" s="6" t="b">
         <f>TRUE</f>
@@ -3936,7 +3953,7 @@
         <v>4</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I60" s="6" t="b">
         <f>TRUE</f>
@@ -3966,7 +3983,7 @@
         <v>4</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I61" s="6" t="b">
         <f>FALSE</f>
@@ -3993,7 +4010,7 @@
         <v>4</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I62" s="6" t="b">
         <f>FALSE</f>
@@ -4020,7 +4037,7 @@
         <v>4</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="I63" s="6" t="b">
         <f>TRUE</f>
@@ -4038,7 +4055,7 @@
     </row>
     <row r="64" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>56</v>
@@ -4050,13 +4067,13 @@
         <v>4</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F64" s="7">
         <v>6</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I64" s="6" t="b">
         <f>TRUE</f>
@@ -4086,10 +4103,10 @@
         <v>6</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I65" s="6" t="b">
         <f>TRUE</f>
@@ -4119,7 +4136,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>196</v>
@@ -4149,7 +4166,7 @@
         <v>5</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>196</v>
@@ -4179,7 +4196,7 @@
         <v>5</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>196</v>
@@ -4209,7 +4226,7 @@
         <v>6</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>242</v>
@@ -4239,7 +4256,7 @@
         <v>6</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>243</v>
@@ -4269,7 +4286,7 @@
         <v>6</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H71" s="6" t="s">
         <v>244</v>
@@ -4299,7 +4316,7 @@
         <v>6</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>241</v>
@@ -4332,7 +4349,7 @@
         <v>6</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H73" s="6" t="s">
         <v>241</v>
@@ -4365,7 +4382,7 @@
         <v>6</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>279</v>
@@ -4395,7 +4412,7 @@
         <v>6</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>279</v>
@@ -4425,7 +4442,7 @@
         <v>6</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>240</v>
@@ -4455,7 +4472,7 @@
         <v>6</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H77" s="6" t="s">
         <v>240</v>
@@ -4485,7 +4502,7 @@
         <v>7</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F78" s="11" t="s">
         <v>232</v>
@@ -4519,7 +4536,7 @@
         <v>7</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F79" s="11" t="s">
         <v>232</v>
@@ -4553,7 +4570,7 @@
         <v>7</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F80" s="11" t="s">
         <v>232</v>
@@ -4587,7 +4604,7 @@
         <v>7</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>239</v>
@@ -4617,7 +4634,7 @@
         <v>7</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>239</v>
@@ -4647,7 +4664,7 @@
         <v>7</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F83" s="12" t="s">
         <v>272</v>
@@ -4681,7 +4698,7 @@
         <v>272</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>273</v>
@@ -4711,7 +4728,7 @@
         <v>7</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F85" s="11" t="s">
         <v>232</v>
@@ -4745,7 +4762,7 @@
         <v>7</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F86" s="11" t="s">
         <v>232</v>
@@ -4779,7 +4796,7 @@
         <v>7</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F87" s="11" t="s">
         <v>232</v>
@@ -4813,7 +4830,7 @@
         <v>7</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H88" s="6" t="s">
         <v>238</v>
@@ -4843,7 +4860,7 @@
         <v>7</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F89" s="12" t="s">
         <v>256</v>
@@ -4877,7 +4894,7 @@
         <v>7</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F90" s="12" t="s">
         <v>256</v>
@@ -4911,7 +4928,7 @@
         <v>7</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F91" s="12" t="s">
         <v>256</v>
@@ -4945,7 +4962,7 @@
         <v>7</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F92" s="12" t="s">
         <v>256</v>
@@ -4979,7 +4996,7 @@
         <v>7</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H93" s="6" t="s">
         <v>236</v>
@@ -5009,7 +5026,7 @@
         <v>7</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H94" s="6" t="s">
         <v>236</v>
@@ -5039,7 +5056,7 @@
         <v>7</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H95" s="6" t="s">
         <v>236</v>
@@ -5069,7 +5086,7 @@
         <v>232</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H96" s="6" t="s">
         <v>235</v>
@@ -5099,7 +5116,7 @@
         <v>232</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>235</v>
@@ -5129,14 +5146,14 @@
         <v>232</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>272</v>
       </c>
       <c r="G98" s="22"/>
       <c r="H98" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I98" s="6" t="b">
         <f>FALSE</f>
@@ -5163,7 +5180,7 @@
         <v>272</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H99" s="6" t="s">
         <v>273</v>
@@ -5193,7 +5210,7 @@
         <v>232</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H100" s="6" t="s">
         <v>278</v>
@@ -5223,7 +5240,7 @@
         <v>232</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H101" s="6" t="s">
         <v>246</v>
@@ -5253,7 +5270,7 @@
         <v>255</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H102" s="6" t="s">
         <v>253</v>
@@ -5283,7 +5300,7 @@
         <v>256</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H103" s="6" t="s">
         <v>258</v>
@@ -5310,7 +5327,7 @@
         <v>256</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H104" s="6" t="s">
         <v>269</v>
@@ -5323,7 +5340,7 @@
         <v>138</v>
       </c>
       <c r="L104" s="6" t="s">
-        <v>214</v>
+        <v>470</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -5340,7 +5357,7 @@
         <v>256</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H105" s="6" t="s">
         <v>269</v>
@@ -5370,7 +5387,7 @@
         <v>256</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H106" s="6" t="s">
         <v>269</v>
@@ -5400,7 +5417,7 @@
         <v>256</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H107" s="6" t="s">
         <v>269</v>
@@ -5413,7 +5430,7 @@
         <v>138</v>
       </c>
       <c r="L107" s="6" t="s">
-        <v>214</v>
+        <v>470</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -5430,7 +5447,7 @@
         <v>324</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H108" s="6" t="s">
         <v>325</v>
@@ -5440,13 +5457,13 @@
         <v>0</v>
       </c>
       <c r="K108" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L108" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>281</v>
       </c>
@@ -5460,7 +5477,7 @@
         <v>324</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H109" s="6" t="s">
         <v>325</v>
@@ -5470,13 +5487,13 @@
         <v>0</v>
       </c>
       <c r="K109" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L109" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>282</v>
       </c>
@@ -5490,7 +5507,7 @@
         <v>324</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H110" s="6" t="s">
         <v>325</v>
@@ -5500,10 +5517,10 @@
         <v>0</v>
       </c>
       <c r="K110" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L110" s="6" t="s">
-        <v>326</v>
+        <v>468</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5520,7 +5537,7 @@
         <v>324</v>
       </c>
       <c r="E111" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H111" s="6" t="s">
         <v>325</v>
@@ -5530,10 +5547,10 @@
         <v>0</v>
       </c>
       <c r="K111" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L111" s="6" t="s">
-        <v>326</v>
+        <v>466</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5550,7 +5567,7 @@
         <v>324</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H112" s="6" t="s">
         <v>325</v>
@@ -5560,10 +5577,10 @@
         <v>0</v>
       </c>
       <c r="K112" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L112" s="6" t="s">
-        <v>326</v>
+        <v>469</v>
       </c>
     </row>
     <row r="113" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5580,7 +5597,7 @@
         <v>324</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H113" s="6" t="s">
         <v>325</v>
@@ -5590,10 +5607,10 @@
         <v>0</v>
       </c>
       <c r="K113" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L113" s="6" t="s">
-        <v>326</v>
+        <v>466</v>
       </c>
     </row>
     <row r="114" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5610,7 +5627,7 @@
         <v>324</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H114" s="6" t="s">
         <v>325</v>
@@ -5620,13 +5637,13 @@
         <v>0</v>
       </c>
       <c r="K114" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L114" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>287</v>
       </c>
@@ -5640,7 +5657,7 @@
         <v>324</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>325</v>
@@ -5650,13 +5667,13 @@
         <v>0</v>
       </c>
       <c r="K115" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L115" s="6" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="116" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>288</v>
       </c>
@@ -5670,7 +5687,7 @@
         <v>324</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H116" s="6" t="s">
         <v>325</v>
@@ -5680,10 +5697,10 @@
         <v>0</v>
       </c>
       <c r="K116" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>326</v>
+        <v>469</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -5700,7 +5717,7 @@
         <v>324</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H117" s="6" t="s">
         <v>325</v>
@@ -5710,10 +5727,10 @@
         <v>0</v>
       </c>
       <c r="K117" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>327</v>
+        <v>467</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5730,7 +5747,7 @@
         <v>324</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H118" s="6" t="s">
         <v>325</v>
@@ -5740,10 +5757,10 @@
         <v>0</v>
       </c>
       <c r="K118" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>327</v>
+        <v>467</v>
       </c>
     </row>
     <row r="119" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5760,7 +5777,7 @@
         <v>324</v>
       </c>
       <c r="E119" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H119" s="6" t="s">
         <v>325</v>
@@ -5770,10 +5787,10 @@
         <v>0</v>
       </c>
       <c r="K119" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L119" s="6" t="s">
-        <v>327</v>
+        <v>467</v>
       </c>
     </row>
     <row r="120" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5790,7 +5807,7 @@
         <v>324</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H120" s="6" t="s">
         <v>325</v>
@@ -5800,10 +5817,10 @@
         <v>0</v>
       </c>
       <c r="K120" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>327</v>
+        <v>467</v>
       </c>
     </row>
     <row r="121" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5820,7 +5837,7 @@
         <v>324</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H121" s="6" t="s">
         <v>325</v>
@@ -5830,10 +5847,10 @@
         <v>0</v>
       </c>
       <c r="K121" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L121" s="6" t="s">
-        <v>327</v>
+        <v>467</v>
       </c>
     </row>
     <row r="122" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -5850,7 +5867,7 @@
         <v>324</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H122" s="6" t="s">
         <v>325</v>
@@ -5860,10 +5877,10 @@
         <v>0</v>
       </c>
       <c r="K122" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>327</v>
+        <v>467</v>
       </c>
     </row>
     <row r="123" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5880,7 +5897,7 @@
         <v>324</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H123" s="6" t="s">
         <v>325</v>
@@ -5890,10 +5907,10 @@
         <v>0</v>
       </c>
       <c r="K123" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L123" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
@@ -5910,7 +5927,7 @@
         <v>324</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H124" s="6" t="s">
         <v>325</v>
@@ -5920,10 +5937,10 @@
         <v>0</v>
       </c>
       <c r="K124" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="125" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5940,7 +5957,7 @@
         <v>324</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H125" s="6" t="s">
         <v>325</v>
@@ -5950,10 +5967,10 @@
         <v>0</v>
       </c>
       <c r="K125" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L125" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="126" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -5970,7 +5987,7 @@
         <v>324</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H126" s="6" t="s">
         <v>325</v>
@@ -5980,10 +5997,10 @@
         <v>0</v>
       </c>
       <c r="K126" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
@@ -6000,7 +6017,7 @@
         <v>324</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H127" s="6" t="s">
         <v>325</v>
@@ -6010,10 +6027,10 @@
         <v>0</v>
       </c>
       <c r="K127" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L127" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="128" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6030,7 +6047,7 @@
         <v>324</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H128" s="6" t="s">
         <v>325</v>
@@ -6040,10 +6057,10 @@
         <v>0</v>
       </c>
       <c r="K128" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="129" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -6060,7 +6077,7 @@
         <v>324</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H129" s="6" t="s">
         <v>325</v>
@@ -6070,30 +6087,30 @@
         <v>0</v>
       </c>
       <c r="K129" s="16" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L129" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B130" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D130" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H130" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I130" s="6" t="b">
         <v>1</v>
@@ -6105,27 +6122,27 @@
         <v>137</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="131" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B131" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D131" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H131" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I131" s="6" t="b">
         <v>1</v>
@@ -6137,27 +6154,27 @@
         <v>137</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B132" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H132" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I132" s="6" t="b">
         <v>1</v>
@@ -6169,27 +6186,27 @@
         <v>137</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A133" s="17" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B133" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D133" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H133" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I133" s="6" t="b">
         <v>1</v>
@@ -6201,27 +6218,27 @@
         <v>137</v>
       </c>
       <c r="L133" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B134" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D134" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H134" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I134" s="6" t="b">
         <v>0</v>
@@ -6235,22 +6252,22 @@
     </row>
     <row r="135" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B135" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D135" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H135" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I135" s="6" t="b">
         <v>0</v>
@@ -6264,22 +6281,22 @@
     </row>
     <row r="136" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B136" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D136" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H136" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I136" s="6" t="b">
         <v>0</v>
@@ -6293,22 +6310,22 @@
     </row>
     <row r="137" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B137" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D137" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H137" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I137" s="6" t="b">
         <v>0</v>
@@ -6322,22 +6339,22 @@
     </row>
     <row r="138" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B138" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D138" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H138" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I138" s="6" t="b">
         <v>0</v>
@@ -6351,22 +6368,22 @@
     </row>
     <row r="139" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A139" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D139" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H139" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I139" s="6" t="b">
         <v>0</v>
@@ -6375,85 +6392,85 @@
         <v>138</v>
       </c>
       <c r="L139" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="140" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B140" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D140" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H140" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="I140" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K140" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="L140" s="6" t="s">
         <v>370</v>
-      </c>
-      <c r="I140" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K140" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="L140" s="6" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="141" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A141" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B141" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D141" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E141" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H141" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="I141" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K141" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="L141" s="6" t="s">
         <v>370</v>
-      </c>
-      <c r="I141" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K141" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="L141" s="6" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="142" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C142" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H142" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I142" s="6" t="b">
         <v>0</v>
@@ -6462,27 +6479,27 @@
         <v>138</v>
       </c>
       <c r="L142" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="143" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B143" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C143" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D143" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H143" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I143" s="6" t="b">
         <v>0</v>
@@ -6491,27 +6508,27 @@
         <v>138</v>
       </c>
       <c r="L143" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B144" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D144" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H144" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I144" s="6" t="b">
         <v>0</v>
@@ -6520,27 +6537,27 @@
         <v>138</v>
       </c>
       <c r="L144" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="145" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B145" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D145" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H145" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I145" s="6" t="b">
         <v>0</v>
@@ -6549,27 +6566,27 @@
         <v>138</v>
       </c>
       <c r="L145" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="146" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B146" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D146" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H146" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I146" s="6" t="b">
         <v>0</v>
@@ -6578,27 +6595,27 @@
         <v>138</v>
       </c>
       <c r="L146" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="147" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B147" s="6" t="s">
         <v>56</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D147" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H147" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I147" s="6" t="b">
         <v>0</v>
@@ -6607,27 +6624,27 @@
         <v>138</v>
       </c>
       <c r="L147" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="148" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D148" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H148" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I148" s="6" t="b">
         <v>0</v>
@@ -6641,22 +6658,22 @@
     </row>
     <row r="149" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D149" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E149" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H149" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I149" s="6" t="b">
         <v>0</v>
@@ -6670,22 +6687,22 @@
     </row>
     <row r="150" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D150" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H150" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I150" s="6" t="b">
         <v>0</v>
@@ -6699,22 +6716,22 @@
     </row>
     <row r="151" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D151" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H151" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I151" s="6" t="b">
         <v>0</v>
@@ -6728,22 +6745,22 @@
     </row>
     <row r="152" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D152" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H152" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I152" s="6" t="b">
         <v>0</v>
@@ -6757,22 +6774,22 @@
     </row>
     <row r="153" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A153" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D153" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H153" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I153" s="6" t="b">
         <v>0</v>
@@ -6786,52 +6803,52 @@
     </row>
     <row r="154" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C154" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D154" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E154" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="H154" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="H154" s="6" t="s">
+      <c r="I154" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K154" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="L154" s="6" t="s">
         <v>407</v>
-      </c>
-      <c r="I154" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="K154" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="L154" s="6" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="155" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B155" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D155" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E155" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="H155" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="H155" s="6" t="s">
-        <v>407</v>
-      </c>
       <c r="I155" s="6" t="b">
         <v>0</v>
       </c>
@@ -6839,28 +6856,28 @@
         <v>138</v>
       </c>
       <c r="L155" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C156" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D156" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E156" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="H156" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="H156" s="6" t="s">
-        <v>407</v>
-      </c>
       <c r="I156" s="6" t="b">
         <v>0</v>
       </c>
@@ -6868,27 +6885,27 @@
         <v>138</v>
       </c>
       <c r="L156" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D157" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E157" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H157" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I157" s="6" t="b">
         <v>0</v>
@@ -6897,27 +6914,27 @@
         <v>137</v>
       </c>
       <c r="L157" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="158" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B158" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D158" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H158" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I158" s="6" t="b">
         <v>0</v>
@@ -6926,27 +6943,27 @@
         <v>137</v>
       </c>
       <c r="L158" s="6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="159" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C159" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D159" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H159" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I159" s="6" t="b">
         <v>0</v>
@@ -6955,27 +6972,27 @@
         <v>137</v>
       </c>
       <c r="L159" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="160" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C160" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D160" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E160" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H160" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I160" s="6" t="b">
         <v>0</v>
@@ -6984,27 +7001,27 @@
         <v>137</v>
       </c>
       <c r="L160" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C161" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D161" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H161" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I161" s="6" t="b">
         <v>0</v>
@@ -7013,27 +7030,27 @@
         <v>137</v>
       </c>
       <c r="L161" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="162" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B162" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C162" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D162" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E162" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H162" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I162" s="6" t="b">
         <v>0</v>
@@ -7042,27 +7059,27 @@
         <v>137</v>
       </c>
       <c r="L162" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C163" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D163" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E163" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H163" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I163" s="6" t="b">
         <v>0</v>
@@ -7071,27 +7088,27 @@
         <v>137</v>
       </c>
       <c r="L163" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="164" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B164" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D164" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H164" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I164" s="6" t="b">
         <v>0</v>
@@ -7100,27 +7117,27 @@
         <v>137</v>
       </c>
       <c r="L164" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="165" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D165" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H165" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I165" s="6" t="b">
         <v>0</v>
@@ -7129,27 +7146,27 @@
         <v>137</v>
       </c>
       <c r="L165" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="166" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D166" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H166" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I166" s="6" t="b">
         <v>0</v>
@@ -7158,27 +7175,27 @@
         <v>137</v>
       </c>
       <c r="L166" s="6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D167" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H167" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I167" s="6" t="b">
         <v>0</v>
@@ -7187,27 +7204,27 @@
         <v>137</v>
       </c>
       <c r="L167" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D168" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H168" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I168" s="6" t="b">
         <v>0</v>
@@ -7216,27 +7233,27 @@
         <v>137</v>
       </c>
       <c r="L168" s="6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="169" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B169" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D169" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E169" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H169" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I169" s="6" t="b">
         <v>0</v>
@@ -7245,27 +7262,27 @@
         <v>137</v>
       </c>
       <c r="L169" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="170" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D170" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E170" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H170" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I170" s="6" t="b">
         <v>0</v>
@@ -7274,27 +7291,27 @@
         <v>137</v>
       </c>
       <c r="L170" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D171" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H171" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I171" s="6" t="b">
         <v>0</v>
@@ -7303,27 +7320,27 @@
         <v>137</v>
       </c>
       <c r="L171" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="172" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D172" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E172" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H172" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I172" s="6" t="b">
         <v>0</v>
@@ -7332,27 +7349,27 @@
         <v>137</v>
       </c>
       <c r="L172" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="173" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A173" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B173" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D173" s="8" t="s">
         <v>324</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H173" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I173" s="6" t="b">
         <v>0</v>
@@ -7361,7 +7378,7 @@
         <v>137</v>
       </c>
       <c r="L173" s="6" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>